<commit_message>
add SPSS file for assignment 3
</commit_message>
<xml_diff>
--- a/OTXData.xlsx
+++ b/OTXData.xlsx
@@ -553,11 +553,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1441647712"/>
-        <c:axId val="-1441647168"/>
+        <c:axId val="-433431840"/>
+        <c:axId val="-433429664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1441647712"/>
+        <c:axId val="-433431840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +600,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1441647168"/>
+        <c:crossAx val="-433429664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -608,7 +608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1441647168"/>
+        <c:axId val="-433429664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +659,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1441647712"/>
+        <c:crossAx val="-433431840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -752,7 +752,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -877,11 +876,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-1441658592"/>
-        <c:axId val="-1441658048"/>
+        <c:axId val="-433429120"/>
+        <c:axId val="-433428032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1441658592"/>
+        <c:axId val="-433429120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,7 +923,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1441658048"/>
+        <c:crossAx val="-433428032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -932,7 +931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1441658048"/>
+        <c:axId val="-433428032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +982,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1441658592"/>
+        <c:crossAx val="-433429120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1185,11 +1184,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-1441661312"/>
-        <c:axId val="-1441653696"/>
+        <c:axId val="-433435104"/>
+        <c:axId val="-433431296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1441661312"/>
+        <c:axId val="-433435104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1232,7 +1231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1441653696"/>
+        <c:crossAx val="-433431296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1240,7 +1239,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1441653696"/>
+        <c:axId val="-433431296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1291,7 +1290,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1441661312"/>
+        <c:crossAx val="-433435104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2977,16 +2976,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3341,10 +3340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3352,644 +3351,965 @@
     <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>32</v>
       </c>
       <c r="B1">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <f>B1/$E$1</f>
+        <v>1.7899894838117826E-4</v>
+      </c>
+      <c r="E1">
+        <f>SUM(B:B)</f>
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>B2/$E$1</f>
+        <v>2.4612355402412009E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>B3/$E$1</f>
+        <v>1.5662407983353099E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f>B4/$E$1</f>
+        <v>8.949947419058913E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <v>728</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>B5/$E$1</f>
+        <v>1.6288904302687222E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
       <c r="B6">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f>B6/$E$1</f>
+        <v>7.3837066207236028E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>35</v>
       </c>
       <c r="B7">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f>B7/$E$1</f>
+        <v>2.0137381692882556E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
       <c r="B8">
         <v>2768</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f>B8/$E$1</f>
+        <v>6.1933636139887678E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
       <c r="B9">
         <v>194</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f>B9/$E$1</f>
+        <v>4.3407244982435729E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>38</v>
       </c>
       <c r="B10">
         <v>143</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>B10/$E$1</f>
+        <v>3.1996062023135615E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11">
         <v>374</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f>B11/$E$1</f>
+        <v>8.368200836820083E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
       <c r="B12">
         <v>555</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f>B12/$E$1</f>
+        <v>1.2418052043944241E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
       <c r="B13">
         <v>190</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>B13/$E$1</f>
+        <v>4.2512250240529835E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
       <c r="B14">
         <v>43</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f>B14/$E$1</f>
+        <v>9.6211934754883313E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15">
         <v>973</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>B15/$E$1</f>
+        <v>2.1770747096860808E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
       <c r="B16">
         <v>269</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f>B16/$E$1</f>
+        <v>6.018839639317119E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>6</v>
       </c>
       <c r="B17">
         <v>5024</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>B17/$E$1</f>
+        <v>0.11241133958337995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
       <c r="B18">
         <v>182</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f>B18/$E$1</f>
+        <v>4.0722260756718056E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>43</v>
       </c>
       <c r="B19">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f>B19/$E$1</f>
+        <v>9.6211934754883313E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
       <c r="B20">
         <v>172</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f>B20/$E$1</f>
+        <v>3.8484773901953325E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
       <c r="B21">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f>B21/$E$1</f>
+        <v>2.4612355402412009E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
       <c r="B22">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f>B22/$E$1</f>
+        <v>2.0361130378359028E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f>B23/$E$1</f>
+        <v>2.2374868547647282E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
       <c r="B24">
         <v>1372</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f>B24/$E$1</f>
+        <v>3.0698319647372071E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25">
         <v>693</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f>B25/$E$1</f>
+        <v>1.5505783903519567E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
       <c r="B26">
         <v>43</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f>B26/$E$1</f>
+        <v>9.6211934754883313E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
       <c r="B27">
         <v>82</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f>B27/$E$1</f>
+        <v>1.8347392209070771E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>49</v>
       </c>
       <c r="B28">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f>B28/$E$1</f>
+        <v>9.6211934754883313E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29">
         <v>183</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f>B29/$E$1</f>
+        <v>4.0946009442194529E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="B30">
         <v>1012</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f>B30/$E$1</f>
+        <v>2.2643366970219049E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
       <c r="B31">
         <v>46</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f>B31/$E$1</f>
+        <v>1.0292439531917751E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
       <c r="B32">
         <v>51</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f>B32/$E$1</f>
+        <v>1.1411182959300114E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
       <c r="B33">
         <v>913</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>B33/$E$1</f>
+        <v>2.042825498400197E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>52</v>
       </c>
       <c r="B34">
         <v>618</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f>B34/$E$1</f>
+        <v>1.3827668762446021E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
       <c r="B35">
         <v>1496</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f>B35/$E$1</f>
+        <v>3.3472803347280332E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>53</v>
       </c>
       <c r="B36">
         <v>104</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f>B36/$E$1</f>
+        <v>2.3269863289553175E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>54</v>
       </c>
       <c r="B37">
         <v>2698</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f>B37/$E$1</f>
+        <v>6.0367395341552367E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
       <c r="B38">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f>B38/$E$1</f>
+        <v>1.6333654039782516E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>56</v>
       </c>
       <c r="B39">
         <v>1495</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f>B39/$E$1</f>
+        <v>3.345042847873269E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>57</v>
       </c>
       <c r="B40">
         <v>108</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f>B40/$E$1</f>
+        <v>2.4164858031459065E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>58</v>
       </c>
       <c r="B41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f>B41/$E$1</f>
+        <v>1.3424921128588369E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>59</v>
       </c>
       <c r="B42">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f>B42/$E$1</f>
+        <v>1.7899894838117826E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>60</v>
       </c>
       <c r="B43">
         <v>189</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f>B43/$E$1</f>
+        <v>4.2288501555053362E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>61</v>
       </c>
       <c r="B44">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f>B44/$E$1</f>
+        <v>1.7228648781688408E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>62</v>
       </c>
       <c r="B45">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f>B45/$E$1</f>
+        <v>4.2512250240529835E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>16</v>
       </c>
       <c r="B46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f>B46/$E$1</f>
+        <v>6.7124605642941847E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>63</v>
       </c>
       <c r="B47">
         <v>94</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <f>B47/$E$1</f>
+        <v>2.1032376434788444E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>64</v>
       </c>
       <c r="B48">
         <v>40</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <f>B48/$E$1</f>
+        <v>8.949947419058913E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>65</v>
       </c>
       <c r="B49">
         <v>156</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <f>B49/$E$1</f>
+        <v>3.4904794934329762E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>66</v>
       </c>
       <c r="B50">
         <v>27</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <f>B50/$E$1</f>
+        <v>6.0412145078647661E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>17</v>
       </c>
       <c r="B51">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <f>B51/$E$1</f>
+        <v>1.9913633007406081E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
       <c r="B52">
         <v>89</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <f>B52/$E$1</f>
+        <v>1.9913633007406081E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>68</v>
       </c>
       <c r="B53">
         <v>36</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <f>B53/$E$1</f>
+        <v>8.0549526771530222E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>69</v>
       </c>
       <c r="B54">
         <v>947</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <f>B54/$E$1</f>
+        <v>2.1189000514621976E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>70</v>
       </c>
       <c r="B55">
         <v>166</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <f>B55/$E$1</f>
+        <v>3.7142281789094489E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>18</v>
       </c>
       <c r="B56">
         <v>48</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <f>B56/$E$1</f>
+        <v>1.0739936902870696E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>19</v>
       </c>
       <c r="B57">
         <v>1556</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <f>B57/$E$1</f>
+        <v>3.4815295460139173E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>71</v>
       </c>
       <c r="B58">
         <v>62</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <f>B58/$E$1</f>
+        <v>1.3872418499541316E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>20</v>
       </c>
       <c r="B59">
         <v>3147</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <f>B59/$E$1</f>
+        <v>7.0413711319446001E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>72</v>
       </c>
       <c r="B60">
         <v>621</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <f>B60/$E$1</f>
+        <v>1.3894793368088963E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
       <c r="B61">
         <v>156</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <f>B61/$E$1</f>
+        <v>3.4904794934329762E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>21</v>
       </c>
       <c r="B62">
         <v>269</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <f>B62/$E$1</f>
+        <v>6.018839639317119E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>74</v>
       </c>
       <c r="B63">
         <v>82</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <f>B63/$E$1</f>
+        <v>1.8347392209070771E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>75</v>
       </c>
       <c r="B64">
         <v>90</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <f>B64/$E$1</f>
+        <v>2.0137381692882554E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>22</v>
       </c>
       <c r="B65">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <f>B65/$E$1</f>
+        <v>1.3872418499541316E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>23</v>
       </c>
       <c r="B66">
         <v>69</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <f>B66/$E$1</f>
+        <v>1.5438659297876624E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>24</v>
       </c>
       <c r="B67">
         <v>633</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <f>B67/$E$1</f>
+        <v>1.4163291790660729E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>76</v>
       </c>
       <c r="B68">
         <v>163</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <f>B68/$E$1</f>
+        <v>3.6471035732665072E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>25</v>
       </c>
       <c r="B69">
         <v>248</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <f>B69/$E$1</f>
+        <v>5.5489673998165264E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>77</v>
       </c>
       <c r="B70">
         <v>50</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <f>B70/$E$1</f>
+        <v>1.118743427382364E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>26</v>
       </c>
       <c r="B71">
         <v>506</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <f>B71/$E$1</f>
+        <v>1.1321683485109525E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>27</v>
       </c>
       <c r="B72">
         <v>1641</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <f>B72/$E$1</f>
+        <v>3.6717159286689192E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
       <c r="B73">
         <v>3859</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <f>B73/$E$1</f>
+        <v>8.6344617725370859E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>78</v>
       </c>
       <c r="B74">
         <v>145</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <f>B74/$E$1</f>
+        <v>3.2443559394088558E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>29</v>
       </c>
       <c r="B75">
         <v>698</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <f>B75/$E$1</f>
+        <v>1.5617658246257804E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>30</v>
       </c>
       <c r="B76">
         <v>3748</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <f>B76/$E$1</f>
+        <v>8.3861007316582012E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>79</v>
       </c>
       <c r="B77">
         <v>107</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <f>B77/$E$1</f>
+        <v>2.3941109345982591E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>80</v>
       </c>
       <c r="B78">
         <v>116</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <f>B78/$E$1</f>
+        <v>2.5954847515270848E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>31</v>
       </c>
       <c r="B79">
         <v>1772</v>
       </c>
+      <c r="C79">
+        <f>B79/$E$1</f>
+        <v>3.9648267066430987E-2</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B79">
-    <sortCondition ref="A36"/>
+  <sortState ref="A1:C79">
+    <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4078,388 +4398,580 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>84</v>
       </c>
       <c r="B1">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <f>B1/$E$1</f>
+        <v>5.9000917792054542E-3</v>
+      </c>
+      <c r="E1">
+        <f>SUM(B:B)</f>
+        <v>7627</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f t="shared" ref="C2:C47" si="0">B2/$E$1</f>
+        <v>7.997902189589616E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
       <c r="B3">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>2.884489314278222E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>7.7356758882915957E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
       <c r="B5">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>5.113412875311394E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.9666972597351512E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="B7">
         <v>102</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1.337354136619903E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f>B8/$E$1</f>
+        <v>8.653467942834666E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
       <c r="B9">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>3.5400550675232724E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>B10/$E$1</f>
+        <v>3.5400550675232724E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11">
         <v>1276</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.16730038022813687</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
         <v>373</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>4.8905205192080768E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13">
         <v>172</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>2.2551461911629735E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14">
         <v>494</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>6.4769896420610984E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15">
         <v>142</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>B15/$E$1</f>
+        <v>1.8618067392159432E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16">
         <v>285</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>3.736724793496788E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
       <c r="B17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f>B17/$E$1</f>
+        <v>6.5556575324505052E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>81</v>
       </c>
       <c r="B18">
         <v>255</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>3.3433853415497573E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>51</v>
       </c>
       <c r="B19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>1.311131506490101E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>82</v>
       </c>
       <c r="B20">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f>B20/$E$1</f>
+        <v>8.653467942834666E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="B21">
         <v>388</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f>B21/$E$1</f>
+        <v>5.0871902451815915E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
       <c r="B22">
         <v>67</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>8.784581093483677E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
       <c r="B23">
         <v>285</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>3.736724793496788E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
       <c r="B24">
         <v>247</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>3.2384948210305492E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
       <c r="B25">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>5.6378654779074338E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
       <c r="B26">
         <v>305</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>3.998951094794808E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>86</v>
       </c>
       <c r="B27">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>3.5400550675232724E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>4.326733971417333E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
       <c r="B29">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1.442244657139111E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
       <c r="B30">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>4.7200734233643635E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
       <c r="B31">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>5.2445260259604042E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>69</v>
       </c>
       <c r="B32">
         <v>178</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>2.3338140815523798E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
       <c r="B33">
         <v>247</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>3.2384948210305492E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>19</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>3.9333945194703029E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>83</v>
       </c>
       <c r="B35">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>7.0801101350465448E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>72</v>
       </c>
       <c r="B36">
         <v>155</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f>B36/$E$1</f>
+        <v>2.0322538350596563E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
       <c r="B37">
         <v>76</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f>B37/$E$1</f>
+        <v>9.9645994493247677E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>23</v>
       </c>
       <c r="B38">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f>B38/$E$1</f>
+        <v>7.4734495869935753E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>25</v>
       </c>
       <c r="B39">
         <v>136</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1.7831388488265373E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>26</v>
       </c>
       <c r="B40">
         <v>25</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>3.2778287662252525E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>87</v>
       </c>
       <c r="B41">
         <v>26</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>3.4089419168742627E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>27</v>
       </c>
       <c r="B42">
         <v>177</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f>B42/$E$1</f>
+        <v>2.3207027664874785E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
       <c r="B43">
         <v>539</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>7.0669988199816444E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>29</v>
       </c>
       <c r="B44">
         <v>102</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>1.337354136619903E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>30</v>
       </c>
       <c r="B45">
         <v>774</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>0.10148157860233381</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>79</v>
       </c>
       <c r="B46">
         <v>36</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>4.7200734233643635E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
       <c r="B47">
         <v>19</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>2.4911498623311919E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4467,6 +4979,7 @@
     <sortCondition descending="1" ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4474,8 +4987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added data for 2017
</commit_message>
<xml_diff>
--- a/OTXData.xlsx
+++ b/OTXData.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="3" r:id="rId1"/>
     <sheet name="2019-2" sheetId="2" r:id="rId2"/>
     <sheet name="2016" sheetId="4" r:id="rId3"/>
     <sheet name="2016-2" sheetId="5" r:id="rId4"/>
+    <sheet name="2017" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="120">
   <si>
     <t>Argentina</t>
   </si>
@@ -291,6 +292,102 @@
   </si>
   <si>
     <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bolivia, Plurinational State of</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Moldova, Republic of</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Zambia</t>
   </si>
 </sst>
 </file>
@@ -553,11 +650,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-433431840"/>
-        <c:axId val="-433429664"/>
+        <c:axId val="1331618544"/>
+        <c:axId val="1331622896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-433431840"/>
+        <c:axId val="1331618544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +697,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-433429664"/>
+        <c:crossAx val="1331622896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -608,7 +705,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-433429664"/>
+        <c:axId val="1331622896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +756,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-433431840"/>
+        <c:crossAx val="1331618544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -876,11 +973,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-433429120"/>
-        <c:axId val="-433428032"/>
+        <c:axId val="1331623440"/>
+        <c:axId val="1331612016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-433429120"/>
+        <c:axId val="1331623440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,7 +1020,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-433428032"/>
+        <c:crossAx val="1331612016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -931,7 +1028,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-433428032"/>
+        <c:axId val="1331612016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -982,7 +1079,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-433429120"/>
+        <c:crossAx val="1331623440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1184,11 +1281,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="-433435104"/>
-        <c:axId val="-433431296"/>
+        <c:axId val="1331621808"/>
+        <c:axId val="1331619632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-433435104"/>
+        <c:axId val="1331621808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,7 +1328,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-433431296"/>
+        <c:crossAx val="1331619632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1239,7 +1336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-433431296"/>
+        <c:axId val="1331619632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1387,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-433435104"/>
+        <c:crossAx val="1331621808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3342,7 +3439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -3359,7 +3456,7 @@
         <v>8</v>
       </c>
       <c r="C1">
-        <f>B1/$E$1</f>
+        <f t="shared" ref="C1:C32" si="0">B1/$E$1</f>
         <v>1.7899894838117826E-4</v>
       </c>
       <c r="E1">
@@ -3375,7 +3472,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <f>B2/$E$1</f>
+        <f t="shared" si="0"/>
         <v>2.4612355402412009E-4</v>
       </c>
     </row>
@@ -3387,7 +3484,7 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <f>B3/$E$1</f>
+        <f t="shared" si="0"/>
         <v>1.5662407983353099E-4</v>
       </c>
     </row>
@@ -3399,7 +3496,7 @@
         <v>40</v>
       </c>
       <c r="C4">
-        <f>B4/$E$1</f>
+        <f t="shared" si="0"/>
         <v>8.949947419058913E-4</v>
       </c>
     </row>
@@ -3411,7 +3508,7 @@
         <v>728</v>
       </c>
       <c r="C5">
-        <f>B5/$E$1</f>
+        <f t="shared" si="0"/>
         <v>1.6288904302687222E-2</v>
       </c>
     </row>
@@ -3423,7 +3520,7 @@
         <v>33</v>
       </c>
       <c r="C6">
-        <f>B6/$E$1</f>
+        <f t="shared" si="0"/>
         <v>7.3837066207236028E-4</v>
       </c>
     </row>
@@ -3435,7 +3532,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <f>B7/$E$1</f>
+        <f t="shared" si="0"/>
         <v>2.0137381692882556E-4</v>
       </c>
     </row>
@@ -3447,7 +3544,7 @@
         <v>2768</v>
       </c>
       <c r="C8">
-        <f>B8/$E$1</f>
+        <f t="shared" si="0"/>
         <v>6.1933636139887678E-2</v>
       </c>
     </row>
@@ -3459,7 +3556,7 @@
         <v>194</v>
       </c>
       <c r="C9">
-        <f>B9/$E$1</f>
+        <f t="shared" si="0"/>
         <v>4.3407244982435729E-3</v>
       </c>
     </row>
@@ -3471,7 +3568,7 @@
         <v>143</v>
       </c>
       <c r="C10">
-        <f>B10/$E$1</f>
+        <f t="shared" si="0"/>
         <v>3.1996062023135615E-3</v>
       </c>
     </row>
@@ -3483,7 +3580,7 @@
         <v>374</v>
       </c>
       <c r="C11">
-        <f>B11/$E$1</f>
+        <f t="shared" si="0"/>
         <v>8.368200836820083E-3</v>
       </c>
     </row>
@@ -3495,7 +3592,7 @@
         <v>555</v>
       </c>
       <c r="C12">
-        <f>B12/$E$1</f>
+        <f t="shared" si="0"/>
         <v>1.2418052043944241E-2</v>
       </c>
     </row>
@@ -3507,7 +3604,7 @@
         <v>190</v>
       </c>
       <c r="C13">
-        <f>B13/$E$1</f>
+        <f t="shared" si="0"/>
         <v>4.2512250240529835E-3</v>
       </c>
     </row>
@@ -3519,7 +3616,7 @@
         <v>43</v>
       </c>
       <c r="C14">
-        <f>B14/$E$1</f>
+        <f t="shared" si="0"/>
         <v>9.6211934754883313E-4</v>
       </c>
     </row>
@@ -3531,7 +3628,7 @@
         <v>973</v>
       </c>
       <c r="C15">
-        <f>B15/$E$1</f>
+        <f t="shared" si="0"/>
         <v>2.1770747096860808E-2</v>
       </c>
     </row>
@@ -3543,7 +3640,7 @@
         <v>269</v>
       </c>
       <c r="C16">
-        <f>B16/$E$1</f>
+        <f t="shared" si="0"/>
         <v>6.018839639317119E-3</v>
       </c>
     </row>
@@ -3555,7 +3652,7 @@
         <v>5024</v>
       </c>
       <c r="C17">
-        <f>B17/$E$1</f>
+        <f t="shared" si="0"/>
         <v>0.11241133958337995</v>
       </c>
     </row>
@@ -3567,7 +3664,7 @@
         <v>182</v>
       </c>
       <c r="C18">
-        <f>B18/$E$1</f>
+        <f t="shared" si="0"/>
         <v>4.0722260756718056E-3</v>
       </c>
     </row>
@@ -3579,7 +3676,7 @@
         <v>43</v>
       </c>
       <c r="C19">
-        <f>B19/$E$1</f>
+        <f t="shared" si="0"/>
         <v>9.6211934754883313E-4</v>
       </c>
     </row>
@@ -3591,7 +3688,7 @@
         <v>172</v>
       </c>
       <c r="C20">
-        <f>B20/$E$1</f>
+        <f t="shared" si="0"/>
         <v>3.8484773901953325E-3</v>
       </c>
     </row>
@@ -3603,7 +3700,7 @@
         <v>11</v>
       </c>
       <c r="C21">
-        <f>B21/$E$1</f>
+        <f t="shared" si="0"/>
         <v>2.4612355402412009E-4</v>
       </c>
     </row>
@@ -3615,7 +3712,7 @@
         <v>91</v>
       </c>
       <c r="C22">
-        <f>B22/$E$1</f>
+        <f t="shared" si="0"/>
         <v>2.0361130378359028E-3</v>
       </c>
     </row>
@@ -3627,7 +3724,7 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <f>B23/$E$1</f>
+        <f t="shared" si="0"/>
         <v>2.2374868547647282E-5</v>
       </c>
     </row>
@@ -3639,7 +3736,7 @@
         <v>1372</v>
       </c>
       <c r="C24">
-        <f>B24/$E$1</f>
+        <f t="shared" si="0"/>
         <v>3.0698319647372071E-2</v>
       </c>
     </row>
@@ -3651,7 +3748,7 @@
         <v>693</v>
       </c>
       <c r="C25">
-        <f>B25/$E$1</f>
+        <f t="shared" si="0"/>
         <v>1.5505783903519567E-2</v>
       </c>
     </row>
@@ -3663,7 +3760,7 @@
         <v>43</v>
       </c>
       <c r="C26">
-        <f>B26/$E$1</f>
+        <f t="shared" si="0"/>
         <v>9.6211934754883313E-4</v>
       </c>
     </row>
@@ -3675,7 +3772,7 @@
         <v>82</v>
       </c>
       <c r="C27">
-        <f>B27/$E$1</f>
+        <f t="shared" si="0"/>
         <v>1.8347392209070771E-3</v>
       </c>
     </row>
@@ -3687,7 +3784,7 @@
         <v>43</v>
       </c>
       <c r="C28">
-        <f>B28/$E$1</f>
+        <f t="shared" si="0"/>
         <v>9.6211934754883313E-4</v>
       </c>
     </row>
@@ -3699,7 +3796,7 @@
         <v>183</v>
       </c>
       <c r="C29">
-        <f>B29/$E$1</f>
+        <f t="shared" si="0"/>
         <v>4.0946009442194529E-3</v>
       </c>
     </row>
@@ -3711,7 +3808,7 @@
         <v>1012</v>
       </c>
       <c r="C30">
-        <f>B30/$E$1</f>
+        <f t="shared" si="0"/>
         <v>2.2643366970219049E-2</v>
       </c>
     </row>
@@ -3723,7 +3820,7 @@
         <v>46</v>
       </c>
       <c r="C31">
-        <f>B31/$E$1</f>
+        <f t="shared" si="0"/>
         <v>1.0292439531917751E-3</v>
       </c>
     </row>
@@ -3735,7 +3832,7 @@
         <v>51</v>
       </c>
       <c r="C32">
-        <f>B32/$E$1</f>
+        <f t="shared" si="0"/>
         <v>1.1411182959300114E-3</v>
       </c>
     </row>
@@ -3747,7 +3844,7 @@
         <v>913</v>
       </c>
       <c r="C33">
-        <f>B33/$E$1</f>
+        <f t="shared" ref="C33:C64" si="1">B33/$E$1</f>
         <v>2.042825498400197E-2</v>
       </c>
     </row>
@@ -3759,7 +3856,7 @@
         <v>618</v>
       </c>
       <c r="C34">
-        <f>B34/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.3827668762446021E-2</v>
       </c>
     </row>
@@ -3771,7 +3868,7 @@
         <v>1496</v>
       </c>
       <c r="C35">
-        <f>B35/$E$1</f>
+        <f t="shared" si="1"/>
         <v>3.3472803347280332E-2</v>
       </c>
     </row>
@@ -3783,7 +3880,7 @@
         <v>104</v>
       </c>
       <c r="C36">
-        <f>B36/$E$1</f>
+        <f t="shared" si="1"/>
         <v>2.3269863289553175E-3</v>
       </c>
     </row>
@@ -3795,7 +3892,7 @@
         <v>2698</v>
       </c>
       <c r="C37">
-        <f>B37/$E$1</f>
+        <f t="shared" si="1"/>
         <v>6.0367395341552367E-2</v>
       </c>
     </row>
@@ -3807,7 +3904,7 @@
         <v>73</v>
       </c>
       <c r="C38">
-        <f>B38/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.6333654039782516E-3</v>
       </c>
     </row>
@@ -3819,7 +3916,7 @@
         <v>1495</v>
       </c>
       <c r="C39">
-        <f>B39/$E$1</f>
+        <f t="shared" si="1"/>
         <v>3.345042847873269E-2</v>
       </c>
     </row>
@@ -3831,7 +3928,7 @@
         <v>108</v>
       </c>
       <c r="C40">
-        <f>B40/$E$1</f>
+        <f t="shared" si="1"/>
         <v>2.4164858031459065E-3</v>
       </c>
     </row>
@@ -3843,7 +3940,7 @@
         <v>6</v>
       </c>
       <c r="C41">
-        <f>B41/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.3424921128588369E-4</v>
       </c>
     </row>
@@ -3855,7 +3952,7 @@
         <v>8</v>
       </c>
       <c r="C42">
-        <f>B42/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.7899894838117826E-4</v>
       </c>
     </row>
@@ -3867,7 +3964,7 @@
         <v>189</v>
       </c>
       <c r="C43">
-        <f>B43/$E$1</f>
+        <f t="shared" si="1"/>
         <v>4.2288501555053362E-3</v>
       </c>
     </row>
@@ -3879,7 +3976,7 @@
         <v>77</v>
       </c>
       <c r="C44">
-        <f>B44/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.7228648781688408E-3</v>
       </c>
     </row>
@@ -3891,7 +3988,7 @@
         <v>19</v>
       </c>
       <c r="C45">
-        <f>B45/$E$1</f>
+        <f t="shared" si="1"/>
         <v>4.2512250240529835E-4</v>
       </c>
     </row>
@@ -3903,7 +4000,7 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <f>B46/$E$1</f>
+        <f t="shared" si="1"/>
         <v>6.7124605642941847E-5</v>
       </c>
     </row>
@@ -3915,7 +4012,7 @@
         <v>94</v>
       </c>
       <c r="C47">
-        <f>B47/$E$1</f>
+        <f t="shared" si="1"/>
         <v>2.1032376434788444E-3</v>
       </c>
     </row>
@@ -3927,7 +4024,7 @@
         <v>40</v>
       </c>
       <c r="C48">
-        <f>B48/$E$1</f>
+        <f t="shared" si="1"/>
         <v>8.949947419058913E-4</v>
       </c>
     </row>
@@ -3939,7 +4036,7 @@
         <v>156</v>
       </c>
       <c r="C49">
-        <f>B49/$E$1</f>
+        <f t="shared" si="1"/>
         <v>3.4904794934329762E-3</v>
       </c>
     </row>
@@ -3951,7 +4048,7 @@
         <v>27</v>
       </c>
       <c r="C50">
-        <f>B50/$E$1</f>
+        <f t="shared" si="1"/>
         <v>6.0412145078647661E-4</v>
       </c>
     </row>
@@ -3963,7 +4060,7 @@
         <v>89</v>
       </c>
       <c r="C51">
-        <f>B51/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.9913633007406081E-3</v>
       </c>
     </row>
@@ -3975,7 +4072,7 @@
         <v>89</v>
       </c>
       <c r="C52">
-        <f>B52/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.9913633007406081E-3</v>
       </c>
     </row>
@@ -3987,7 +4084,7 @@
         <v>36</v>
       </c>
       <c r="C53">
-        <f>B53/$E$1</f>
+        <f t="shared" si="1"/>
         <v>8.0549526771530222E-4</v>
       </c>
     </row>
@@ -3999,7 +4096,7 @@
         <v>947</v>
       </c>
       <c r="C54">
-        <f>B54/$E$1</f>
+        <f t="shared" si="1"/>
         <v>2.1189000514621976E-2</v>
       </c>
     </row>
@@ -4011,7 +4108,7 @@
         <v>166</v>
       </c>
       <c r="C55">
-        <f>B55/$E$1</f>
+        <f t="shared" si="1"/>
         <v>3.7142281789094489E-3</v>
       </c>
     </row>
@@ -4023,7 +4120,7 @@
         <v>48</v>
       </c>
       <c r="C56">
-        <f>B56/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.0739936902870696E-3</v>
       </c>
     </row>
@@ -4035,7 +4132,7 @@
         <v>1556</v>
       </c>
       <c r="C57">
-        <f>B57/$E$1</f>
+        <f t="shared" si="1"/>
         <v>3.4815295460139173E-2</v>
       </c>
     </row>
@@ -4047,7 +4144,7 @@
         <v>62</v>
       </c>
       <c r="C58">
-        <f>B58/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.3872418499541316E-3</v>
       </c>
     </row>
@@ -4059,7 +4156,7 @@
         <v>3147</v>
       </c>
       <c r="C59">
-        <f>B59/$E$1</f>
+        <f t="shared" si="1"/>
         <v>7.0413711319446001E-2</v>
       </c>
     </row>
@@ -4071,7 +4168,7 @@
         <v>621</v>
       </c>
       <c r="C60">
-        <f>B60/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.3894793368088963E-2</v>
       </c>
     </row>
@@ -4083,7 +4180,7 @@
         <v>156</v>
       </c>
       <c r="C61">
-        <f>B61/$E$1</f>
+        <f t="shared" si="1"/>
         <v>3.4904794934329762E-3</v>
       </c>
     </row>
@@ -4095,7 +4192,7 @@
         <v>269</v>
       </c>
       <c r="C62">
-        <f>B62/$E$1</f>
+        <f t="shared" si="1"/>
         <v>6.018839639317119E-3</v>
       </c>
     </row>
@@ -4107,7 +4204,7 @@
         <v>82</v>
       </c>
       <c r="C63">
-        <f>B63/$E$1</f>
+        <f t="shared" si="1"/>
         <v>1.8347392209070771E-3</v>
       </c>
     </row>
@@ -4119,7 +4216,7 @@
         <v>90</v>
       </c>
       <c r="C64">
-        <f>B64/$E$1</f>
+        <f t="shared" si="1"/>
         <v>2.0137381692882554E-3</v>
       </c>
     </row>
@@ -4131,7 +4228,7 @@
         <v>62</v>
       </c>
       <c r="C65">
-        <f>B65/$E$1</f>
+        <f t="shared" ref="C65:C96" si="2">B65/$E$1</f>
         <v>1.3872418499541316E-3</v>
       </c>
     </row>
@@ -4143,7 +4240,7 @@
         <v>69</v>
       </c>
       <c r="C66">
-        <f>B66/$E$1</f>
+        <f t="shared" si="2"/>
         <v>1.5438659297876624E-3</v>
       </c>
     </row>
@@ -4155,7 +4252,7 @@
         <v>633</v>
       </c>
       <c r="C67">
-        <f>B67/$E$1</f>
+        <f t="shared" si="2"/>
         <v>1.4163291790660729E-2</v>
       </c>
     </row>
@@ -4167,7 +4264,7 @@
         <v>163</v>
       </c>
       <c r="C68">
-        <f>B68/$E$1</f>
+        <f t="shared" si="2"/>
         <v>3.6471035732665072E-3</v>
       </c>
     </row>
@@ -4179,7 +4276,7 @@
         <v>248</v>
       </c>
       <c r="C69">
-        <f>B69/$E$1</f>
+        <f t="shared" si="2"/>
         <v>5.5489673998165264E-3</v>
       </c>
     </row>
@@ -4191,7 +4288,7 @@
         <v>50</v>
       </c>
       <c r="C70">
-        <f>B70/$E$1</f>
+        <f t="shared" si="2"/>
         <v>1.118743427382364E-3</v>
       </c>
     </row>
@@ -4203,7 +4300,7 @@
         <v>506</v>
       </c>
       <c r="C71">
-        <f>B71/$E$1</f>
+        <f t="shared" si="2"/>
         <v>1.1321683485109525E-2</v>
       </c>
     </row>
@@ -4215,7 +4312,7 @@
         <v>1641</v>
       </c>
       <c r="C72">
-        <f>B72/$E$1</f>
+        <f t="shared" si="2"/>
         <v>3.6717159286689192E-2</v>
       </c>
     </row>
@@ -4227,7 +4324,7 @@
         <v>3859</v>
       </c>
       <c r="C73">
-        <f>B73/$E$1</f>
+        <f t="shared" si="2"/>
         <v>8.6344617725370859E-2</v>
       </c>
     </row>
@@ -4239,7 +4336,7 @@
         <v>145</v>
       </c>
       <c r="C74">
-        <f>B74/$E$1</f>
+        <f t="shared" si="2"/>
         <v>3.2443559394088558E-3</v>
       </c>
     </row>
@@ -4251,7 +4348,7 @@
         <v>698</v>
       </c>
       <c r="C75">
-        <f>B75/$E$1</f>
+        <f t="shared" si="2"/>
         <v>1.5617658246257804E-2</v>
       </c>
     </row>
@@ -4263,7 +4360,7 @@
         <v>3748</v>
       </c>
       <c r="C76">
-        <f>B76/$E$1</f>
+        <f t="shared" si="2"/>
         <v>8.3861007316582012E-2</v>
       </c>
     </row>
@@ -4275,7 +4372,7 @@
         <v>107</v>
       </c>
       <c r="C77">
-        <f>B77/$E$1</f>
+        <f t="shared" si="2"/>
         <v>2.3941109345982591E-3</v>
       </c>
     </row>
@@ -4287,7 +4384,7 @@
         <v>116</v>
       </c>
       <c r="C78">
-        <f>B78/$E$1</f>
+        <f t="shared" si="2"/>
         <v>2.5954847515270848E-3</v>
       </c>
     </row>
@@ -4299,7 +4396,7 @@
         <v>1772</v>
       </c>
       <c r="C79">
-        <f>B79/$E$1</f>
+        <f t="shared" si="2"/>
         <v>3.9648267066430987E-2</v>
       </c>
     </row>
@@ -4987,7 +5084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -5048,4 +5145,1239 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1">
+        <v>67</v>
+      </c>
+      <c r="C1">
+        <f>B1/$E$1</f>
+        <v>1.4051718713953146E-3</v>
+      </c>
+      <c r="E1">
+        <f>SUM(B:B)</f>
+        <v>47681</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>67</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C65" si="0">B2/$E$1</f>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>930</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>1.9504624483546906E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>172</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>3.6073068937312555E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1676</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3.5150269499381305E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.0905811539187516E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>4.1945428996875066E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>6.5015414945156355E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f>B9/$E$1</f>
+        <v>1.0486357249218766E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10">
+        <v>215</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>4.5091336171640692E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <f>B11/$E$1</f>
+        <v>3.9848157547031312E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12">
+        <v>75</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1.5729535873828149E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>1848</v>
+      </c>
+      <c r="C13">
+        <f>B13/$E$1</f>
+        <v>3.8757576393112558E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>238</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>4.9915060506281325E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1.8875443048593779E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16">
+        <v>67</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>49</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>1.0276630104234391E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>1721</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>3.6094041651810994E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19">
+        <v>67</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <v>1561</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>3.2738407332060987E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>86</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>1.8036534468656277E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22">
+        <v>802</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>1.6820117027746901E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23">
+        <v>75</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>1.5729535873828149E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24">
+        <v>111</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>2.327971309326566E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25">
+        <v>67</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>1.5729535873828149E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27">
+        <v>85</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>1.7826807323671904E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>319</v>
+      </c>
+      <c r="C28">
+        <f>B28/$E$1</f>
+        <v>6.6902959250015734E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29">
+        <v>802</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>1.6820117027746901E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>3.7750886097187559E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>3.7750886097187559E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>1638</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>3.4353306348440679E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>1810</v>
+      </c>
+      <c r="C33">
+        <f>B33/$E$1</f>
+        <v>3.7960613242171933E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34">
+        <v>296</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>6.2079234915375101E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>440</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>9.2279943793125152E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36">
+        <v>68</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>1.4261445858937522E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37">
+        <v>877</v>
+      </c>
+      <c r="C37">
+        <f>B37/$E$1</f>
+        <v>1.8393070615129715E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>662</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>1.3883936997965647E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39">
+        <v>67</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>2193</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>4.5993162895073512E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41">
+        <v>139</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>2.9152073152828172E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42">
+        <v>71</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>1.4890627293890648E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43">
+        <v>359</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>7.5292045049390743E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44">
+        <v>52</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>1.0905811539187516E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45">
+        <v>1578</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>3.3094943478534429E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46">
+        <v>408</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>8.5568675153625141E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <v>2765</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>5.7989555588179781E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48">
+        <v>20</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>4.1945428996875066E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49">
+        <v>139</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>2.9152073152828172E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50">
+        <v>218</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>4.5720517606593824E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51">
+        <v>96</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>2.013380591850003E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52">
+        <v>160</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>3.3556343197500053E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53">
+        <v>42</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>8.8085400893437638E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54">
+        <v>49</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>1.0276630104234391E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55">
+        <v>67</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56">
+        <v>149</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>3.1249344602671922E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57">
+        <v>11</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>2.3069985948281286E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58">
+        <v>25</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>5.2431786246093833E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59">
+        <v>29</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>6.0820872045468848E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60">
+        <v>187</v>
+      </c>
+      <c r="C60">
+        <f>B60/$E$1</f>
+        <v>3.9218976112078184E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61">
+        <v>1154</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>2.4202512531196912E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62">
+        <v>42</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>8.8085400893437638E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63">
+        <v>31</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>6.5015414945156355E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64">
+        <v>67</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65">
+        <v>28</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>5.8723600595625089E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66">
+        <v>33</v>
+      </c>
+      <c r="C66">
+        <f t="shared" ref="C66:C101" si="1">B66/$E$1</f>
+        <v>6.9209957844843862E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>109</v>
+      </c>
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="1"/>
+        <v>1.0486357249218766E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>79</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>1.656844445376565E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69">
+        <v>75</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>1.5729535873828149E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70">
+        <v>18</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>3.7750886097187559E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>146</v>
+      </c>
+      <c r="C71">
+        <f>B71/$E$1</f>
+        <v>3.0620163167718799E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>196</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>4.1106520416937563E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>112</v>
+      </c>
+      <c r="B73">
+        <v>89</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>1.8665715903609405E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>18</v>
+      </c>
+      <c r="B74">
+        <v>215</v>
+      </c>
+      <c r="C74">
+        <f>B74/$E$1</f>
+        <v>4.5091336171640692E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>19</v>
+      </c>
+      <c r="B75">
+        <v>218</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>4.5720517606593824E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76">
+        <v>67</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77">
+        <v>195</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>4.0896793271953192E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>113</v>
+      </c>
+      <c r="B78">
+        <v>67</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>1.4051718713953146E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79">
+        <v>1258</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>2.6383674839034418E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>114</v>
+      </c>
+      <c r="B80">
+        <v>18</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>3.7750886097187559E-4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>72</v>
+      </c>
+      <c r="B81">
+        <v>1073</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>2.2503722656823474E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82">
+        <v>18</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>3.7750886097187559E-4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>21</v>
+      </c>
+      <c r="B83">
+        <v>27</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>5.6626329145781341E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>115</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>1.8875443048593779E-4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B85">
+        <v>1638</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>3.4353306348440679E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86">
+        <v>110</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>2.3069985948281288E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>116</v>
+      </c>
+      <c r="B87">
+        <v>141</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>2.9571527442796919E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88">
+        <v>1670</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>3.5024433212390682E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89">
+        <v>1974</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>4.1400138419915689E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>25</v>
+      </c>
+      <c r="B90">
+        <v>863</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>1.8099452612151592E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>26</v>
+      </c>
+      <c r="B91">
+        <v>1897</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>3.9785239403535996E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>117</v>
+      </c>
+      <c r="B92">
+        <v>35</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>7.3404500744531369E-4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93">
+        <v>489</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>1.0255657389735953E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94">
+        <v>1087</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>2.2797340659801598E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>78</v>
+      </c>
+      <c r="B95">
+        <v>641</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>1.3443509993498458E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>29</v>
+      </c>
+      <c r="B96">
+        <v>2074</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>4.3497409869759446E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>30</v>
+      </c>
+      <c r="B97">
+        <v>3334</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>6.9923030137790734E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98">
+        <v>16</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>3.3556343197500051E-4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99">
+        <v>74</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>1.5519808728843775E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>31</v>
+      </c>
+      <c r="B100">
+        <v>488</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>1.0234684675237516E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101">
+        <v>60</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>1.2583628699062519E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added overview spreadsheet to Excel file
</commit_message>
<xml_diff>
--- a/OTXData.xlsx
+++ b/OTXData.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11475"/>
   </bookViews>
   <sheets>
-    <sheet name="2019" sheetId="3" r:id="rId1"/>
-    <sheet name="2019-2" sheetId="2" r:id="rId2"/>
-    <sheet name="2016" sheetId="4" r:id="rId3"/>
-    <sheet name="2016-2" sheetId="5" r:id="rId4"/>
-    <sheet name="2017" sheetId="6" r:id="rId5"/>
+    <sheet name="ALL" sheetId="7" r:id="rId1"/>
+    <sheet name="2019" sheetId="3" r:id="rId2"/>
+    <sheet name="2019-2" sheetId="2" r:id="rId3"/>
+    <sheet name="2016" sheetId="4" r:id="rId4"/>
+    <sheet name="2016-2" sheetId="5" r:id="rId5"/>
+    <sheet name="2017" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="137">
   <si>
     <t>Argentina</t>
   </si>
@@ -388,6 +389,57 @@
   </si>
   <si>
     <t>Zambia</t>
+  </si>
+  <si>
+    <t>Azerbijan</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Korea, Democratic People'</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic R</t>
+  </si>
+  <si>
+    <t>Venezuela, Bolivarian Rep</t>
+  </si>
+  <si>
+    <t>Countryname</t>
+  </si>
+  <si>
+    <t>PercentageOTX2016</t>
+  </si>
+  <si>
+    <t>PercentageSource2019</t>
+  </si>
+  <si>
+    <t>PercentageOTX2019</t>
+  </si>
+  <si>
+    <t>CostsSource2016</t>
+  </si>
+  <si>
+    <t>RansomwareOTX2019</t>
+  </si>
+  <si>
+    <t>MalwareOTX2019</t>
+  </si>
+  <si>
+    <t>RansomwareSource2019</t>
+  </si>
+  <si>
+    <t>MlwareSource2019</t>
+  </si>
+  <si>
+    <t>PercentageOTX2017</t>
+  </si>
+  <si>
+    <t>VictimsSource2017</t>
   </si>
 </sst>
 </file>
@@ -482,7 +534,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -650,11 +701,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1331618544"/>
-        <c:axId val="1331622896"/>
+        <c:axId val="-605562928"/>
+        <c:axId val="-605559120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1331618544"/>
+        <c:axId val="-605562928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,7 +748,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1331622896"/>
+        <c:crossAx val="-605559120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -705,7 +756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1331622896"/>
+        <c:axId val="-605559120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -756,7 +807,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1331618544"/>
+        <c:crossAx val="-605562928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -973,11 +1024,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="1331623440"/>
-        <c:axId val="1331612016"/>
+        <c:axId val="-605552592"/>
+        <c:axId val="-605550960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1331623440"/>
+        <c:axId val="-605552592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1020,7 +1071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1331612016"/>
+        <c:crossAx val="-605550960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1028,7 +1079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1331612016"/>
+        <c:axId val="-605550960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1079,7 +1130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1331623440"/>
+        <c:crossAx val="-605552592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1168,7 +1219,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1281,11 +1331,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="1331621808"/>
-        <c:axId val="1331619632"/>
+        <c:axId val="-605554768"/>
+        <c:axId val="-605552048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1331621808"/>
+        <c:axId val="-605554768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1378,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1331619632"/>
+        <c:crossAx val="-605552048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1336,7 +1386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1331619632"/>
+        <c:axId val="-605552048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,7 +1437,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1331621808"/>
+        <c:crossAx val="-605554768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3437,6 +3487,1345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>1.7899999999999999E-4</v>
+      </c>
+      <c r="H2">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I2">
+        <v>1.8</v>
+      </c>
+      <c r="J2">
+        <v>1.4051999999999999E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>2.4612000000000001E-4</v>
+      </c>
+      <c r="J3">
+        <v>1.4051999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4">
+        <v>5.9000900000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1.5662E-4</v>
+      </c>
+      <c r="J5">
+        <v>1.95046E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>8.9499999999999996E-4</v>
+      </c>
+      <c r="D6">
+        <v>7.9979000000000005E-3</v>
+      </c>
+      <c r="J6">
+        <v>3.6072999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1.6288899999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>7.73568E-3</v>
+      </c>
+      <c r="E7">
+        <v>4.3</v>
+      </c>
+      <c r="J7">
+        <v>3.5150300000000002E-2</v>
+      </c>
+      <c r="K7">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>7.3837000000000002E-4</v>
+      </c>
+      <c r="D8">
+        <v>7.73568E-3</v>
+      </c>
+      <c r="J8">
+        <v>1.0905999999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9">
+        <v>4.1950000000000001E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>2.0137E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>1.9667E-3</v>
+      </c>
+      <c r="H11">
+        <v>13.78</v>
+      </c>
+      <c r="J11">
+        <v>1.049E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>6.1933639999999998E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.2452</v>
+      </c>
+      <c r="J12">
+        <v>4.5091000000000003E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>4.3407200000000002E-3</v>
+      </c>
+      <c r="D13">
+        <v>1.337354E-2</v>
+      </c>
+      <c r="I13">
+        <v>2.8</v>
+      </c>
+      <c r="J13">
+        <v>3.9849999999999998E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14">
+        <v>1.573E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15">
+        <v>3.1996099999999999E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>8.3681999999999993E-3</v>
+      </c>
+      <c r="D16">
+        <v>8.6534699999999999E-3</v>
+      </c>
+      <c r="E16">
+        <v>5.21</v>
+      </c>
+      <c r="G16">
+        <v>95</v>
+      </c>
+      <c r="J16">
+        <v>3.8757600000000003E-2</v>
+      </c>
+      <c r="K16">
+        <v>62.21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17">
+        <v>4.2512299999999999E-3</v>
+      </c>
+      <c r="G17">
+        <v>17</v>
+      </c>
+      <c r="J17">
+        <v>1.0277000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18">
+        <v>9.6212000000000001E-4</v>
+      </c>
+      <c r="I18">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2.1770749999999998E-2</v>
+      </c>
+      <c r="D19">
+        <v>3.5400599999999998E-3</v>
+      </c>
+      <c r="F19">
+        <v>277</v>
+      </c>
+      <c r="J19">
+        <v>3.6094000000000001E-2</v>
+      </c>
+      <c r="K19">
+        <v>10.14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20">
+        <v>6.0188400000000001E-3</v>
+      </c>
+      <c r="J20">
+        <v>1.4051999999999999E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>0.11241134</v>
+      </c>
+      <c r="D21">
+        <v>0.16730038</v>
+      </c>
+      <c r="F21">
+        <v>31</v>
+      </c>
+      <c r="G21">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>1.94</v>
+      </c>
+      <c r="I21">
+        <v>2.4</v>
+      </c>
+      <c r="J21">
+        <v>3.2738400000000001E-2</v>
+      </c>
+      <c r="K21">
+        <v>352.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <v>4.0722299999999996E-3</v>
+      </c>
+      <c r="J22">
+        <v>1.8037000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23">
+        <v>9.6212000000000001E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24">
+        <v>3.84848E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="J25">
+        <v>1.573E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26">
+        <v>2.4612000000000001E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="J27">
+        <v>2.3280000000000002E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="J28">
+        <v>1.4051999999999999E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>2.0361099999999998E-3</v>
+      </c>
+      <c r="D29">
+        <v>4.8905209999999998E-2</v>
+      </c>
+      <c r="J29">
+        <v>6.6902999999999997E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30">
+        <v>2.2370000000000001E-5</v>
+      </c>
+      <c r="J30">
+        <v>3.4353300000000003E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>3.0698320000000001E-2</v>
+      </c>
+      <c r="C31">
+        <v>0.21990000000000001</v>
+      </c>
+      <c r="D31">
+        <v>2.2551459999999999E-2</v>
+      </c>
+      <c r="J31">
+        <v>3.7960599999999997E-2</v>
+      </c>
+      <c r="K31">
+        <v>19.309999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>1.550578E-2</v>
+      </c>
+      <c r="D32">
+        <v>6.4769900000000005E-2</v>
+      </c>
+      <c r="E32">
+        <v>7.84</v>
+      </c>
+      <c r="J32">
+        <v>9.2280000000000001E-3</v>
+      </c>
+      <c r="K32">
+        <v>23.36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>9.6212000000000001E-4</v>
+      </c>
+      <c r="G33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34">
+        <v>1.8347400000000001E-3</v>
+      </c>
+      <c r="J34">
+        <v>1.8393099999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>9.6212000000000001E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="J36">
+        <v>1.4261E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>4.0946000000000003E-3</v>
+      </c>
+      <c r="D37">
+        <v>1.861807E-2</v>
+      </c>
+      <c r="J37">
+        <v>1.3883899999999999E-2</v>
+      </c>
+      <c r="K37">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>2.2643369999999999E-2</v>
+      </c>
+      <c r="D38">
+        <v>3.7367249999999998E-2</v>
+      </c>
+      <c r="F38">
+        <v>277</v>
+      </c>
+      <c r="G38">
+        <v>144</v>
+      </c>
+      <c r="H38">
+        <v>1.91</v>
+      </c>
+      <c r="J38">
+        <v>4.5993199999999998E-2</v>
+      </c>
+      <c r="K38">
+        <v>186.44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39">
+        <v>1.0292400000000001E-3</v>
+      </c>
+      <c r="D39">
+        <v>6.5556999999999996E-4</v>
+      </c>
+      <c r="J39">
+        <v>2.9152000000000002E-3</v>
+      </c>
+      <c r="K39">
+        <v>59.45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>122</v>
+      </c>
+      <c r="D40">
+        <v>3.3433850000000001E-2</v>
+      </c>
+      <c r="J40">
+        <v>1.4890999999999999E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>51</v>
+      </c>
+      <c r="B41">
+        <v>1.14112E-3</v>
+      </c>
+      <c r="D41">
+        <v>1.31113E-3</v>
+      </c>
+      <c r="J41">
+        <v>7.5291999999999998E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42">
+        <v>8.6534699999999999E-3</v>
+      </c>
+      <c r="J42">
+        <v>1.0905999999999999E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43">
+        <v>2.042826E-2</v>
+      </c>
+      <c r="D43">
+        <v>5.0871899999999998E-2</v>
+      </c>
+      <c r="J43">
+        <v>3.3094899999999997E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44">
+        <v>1.382767E-2</v>
+      </c>
+      <c r="C44">
+        <v>0.21959999999999999</v>
+      </c>
+      <c r="D44">
+        <v>8.7845800000000002E-3</v>
+      </c>
+      <c r="G44">
+        <v>22</v>
+      </c>
+      <c r="J44">
+        <v>8.5568999999999992E-3</v>
+      </c>
+      <c r="K44">
+        <v>16.440000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45">
+        <v>3.3472799999999997E-2</v>
+      </c>
+      <c r="D45">
+        <v>3.7367249999999998E-2</v>
+      </c>
+      <c r="E45">
+        <v>8.39</v>
+      </c>
+      <c r="F45">
+        <v>343</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="J45">
+        <v>5.7989600000000002E-2</v>
+      </c>
+      <c r="K45">
+        <v>17.739999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46">
+        <v>2.3269900000000001E-3</v>
+      </c>
+      <c r="D46">
+        <v>3.2384950000000003E-2</v>
+      </c>
+      <c r="J46">
+        <v>4.1950000000000001E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47">
+        <v>6.0367400000000002E-2</v>
+      </c>
+      <c r="D47">
+        <v>5.6378699999999997E-3</v>
+      </c>
+      <c r="J47">
+        <v>2.9152000000000002E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48">
+        <v>1.6333700000000001E-3</v>
+      </c>
+      <c r="F48">
+        <v>31</v>
+      </c>
+      <c r="G48">
+        <v>11</v>
+      </c>
+      <c r="J48">
+        <v>4.5720999999999999E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49">
+        <v>3.3450430000000003E-2</v>
+      </c>
+      <c r="F49">
+        <v>18</v>
+      </c>
+      <c r="G49">
+        <v>22</v>
+      </c>
+      <c r="I49">
+        <v>2.6</v>
+      </c>
+      <c r="J49">
+        <v>2.0133999999999998E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50">
+        <v>2.4164899999999999E-3</v>
+      </c>
+      <c r="J50">
+        <v>3.3555999999999998E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51">
+        <v>1.3425000000000001E-4</v>
+      </c>
+      <c r="J51">
+        <v>8.809E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>124</v>
+      </c>
+      <c r="B52">
+        <v>1.7899999999999999E-4</v>
+      </c>
+      <c r="G52">
+        <v>8</v>
+      </c>
+      <c r="J52">
+        <v>1.0277000000000001E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53">
+        <v>4.2288500000000001E-3</v>
+      </c>
+      <c r="J53">
+        <v>3.1248999999999999E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54">
+        <v>1.72287E-3</v>
+      </c>
+      <c r="D54">
+        <v>3.9989509999999999E-2</v>
+      </c>
+      <c r="J54">
+        <v>2.307E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B56">
+        <v>4.2512000000000002E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57">
+        <v>6.7119999999999994E-5</v>
+      </c>
+      <c r="J57">
+        <v>3.9218999999999999E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58">
+        <v>2.1032400000000001E-3</v>
+      </c>
+      <c r="D58">
+        <v>1.44225E-3</v>
+      </c>
+      <c r="J58">
+        <v>2.4202499999999998E-2</v>
+      </c>
+      <c r="K58">
+        <v>33.15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59">
+        <v>8.9499999999999996E-4</v>
+      </c>
+      <c r="C59">
+        <v>0.24049999999999999</v>
+      </c>
+      <c r="D59">
+        <v>4.7200699999999998E-3</v>
+      </c>
+      <c r="J59">
+        <v>6.5019999999999998E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60">
+        <v>3.4904799999999998E-3</v>
+      </c>
+      <c r="J60">
+        <v>1.4051999999999999E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61">
+        <v>6.0411999999999998E-4</v>
+      </c>
+      <c r="C61">
+        <v>0.2387</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62">
+        <v>1.9913600000000002E-3</v>
+      </c>
+      <c r="D62">
+        <v>5.2445299999999999E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63">
+        <v>1.9913600000000002E-3</v>
+      </c>
+      <c r="J63">
+        <v>1.6567999999999999E-3</v>
+      </c>
+      <c r="K63">
+        <v>3.43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64">
+        <v>8.0550000000000001E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65">
+        <v>2.1189E-2</v>
+      </c>
+      <c r="D65">
+        <v>2.333814E-2</v>
+      </c>
+      <c r="G65">
+        <v>9</v>
+      </c>
+      <c r="J65">
+        <v>3.0620000000000001E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66">
+        <v>3.7142299999999998E-3</v>
+      </c>
+      <c r="D66">
+        <v>3.2384950000000003E-2</v>
+      </c>
+      <c r="G66">
+        <v>13</v>
+      </c>
+      <c r="J66">
+        <v>4.1107000000000001E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>18</v>
+      </c>
+      <c r="B67">
+        <v>1.0739899999999999E-3</v>
+      </c>
+      <c r="C67">
+        <v>0.2389</v>
+      </c>
+      <c r="G67">
+        <v>8</v>
+      </c>
+      <c r="J67">
+        <v>4.5091000000000003E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68">
+        <v>3.48153E-2</v>
+      </c>
+      <c r="C68">
+        <v>0.24129999999999999</v>
+      </c>
+      <c r="D68">
+        <v>3.9334E-4</v>
+      </c>
+      <c r="G68">
+        <v>6</v>
+      </c>
+      <c r="J68">
+        <v>4.5720999999999999E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69">
+        <v>1.3872400000000001E-3</v>
+      </c>
+      <c r="C69">
+        <v>0.21970000000000001</v>
+      </c>
+      <c r="J69">
+        <v>1.4051999999999999E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70">
+        <v>7.0801099999999997E-3</v>
+      </c>
+      <c r="J70">
+        <v>4.0896999999999999E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71">
+        <v>7.0413710000000004E-2</v>
+      </c>
+      <c r="G71">
+        <v>137</v>
+      </c>
+      <c r="J71">
+        <v>2.63837E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72">
+        <v>1.3894790000000001E-2</v>
+      </c>
+      <c r="D72">
+        <v>2.032254E-2</v>
+      </c>
+      <c r="J72">
+        <v>2.2503700000000001E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73">
+        <v>3.4904799999999998E-3</v>
+      </c>
+      <c r="C73">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="I73">
+        <v>1.9</v>
+      </c>
+      <c r="J73">
+        <v>3.7750000000000001E-4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74">
+        <v>6.0188400000000001E-3</v>
+      </c>
+      <c r="F74">
+        <v>35</v>
+      </c>
+      <c r="J74">
+        <v>5.6630000000000005E-4</v>
+      </c>
+      <c r="K74">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>1.8347400000000001E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>2.01374E-3</v>
+      </c>
+      <c r="J76">
+        <v>3.4353300000000003E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77">
+        <v>1.3872400000000001E-3</v>
+      </c>
+      <c r="D77">
+        <v>9.9646000000000005E-3</v>
+      </c>
+      <c r="J77">
+        <v>2.307E-3</v>
+      </c>
+      <c r="K77">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>23</v>
+      </c>
+      <c r="B78">
+        <v>1.5438699999999999E-3</v>
+      </c>
+      <c r="D78">
+        <v>7.4734500000000004E-3</v>
+      </c>
+      <c r="F78">
+        <v>35</v>
+      </c>
+      <c r="J78">
+        <v>3.5024399999999997E-2</v>
+      </c>
+      <c r="K78">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79">
+        <v>1.416329E-2</v>
+      </c>
+      <c r="F79">
+        <v>7</v>
+      </c>
+      <c r="J79">
+        <v>4.1400100000000002E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>76</v>
+      </c>
+      <c r="B80">
+        <v>3.6470999999999999E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81">
+        <v>5.5489700000000003E-3</v>
+      </c>
+      <c r="C81">
+        <v>0.2213</v>
+      </c>
+      <c r="D81">
+        <v>1.7831389999999999E-2</v>
+      </c>
+      <c r="J81">
+        <v>1.8099500000000001E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>77</v>
+      </c>
+      <c r="B82">
+        <v>1.11874E-3</v>
+      </c>
+      <c r="G82">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83">
+        <v>1.1321680000000001E-2</v>
+      </c>
+      <c r="D83">
+        <v>3.2778299999999998E-3</v>
+      </c>
+      <c r="F83">
+        <v>277</v>
+      </c>
+      <c r="G83">
+        <v>14</v>
+      </c>
+      <c r="J83">
+        <v>3.97852E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>27</v>
+      </c>
+      <c r="B84">
+        <v>3.6717159999999999E-2</v>
+      </c>
+      <c r="D84">
+        <v>2.320703E-2</v>
+      </c>
+      <c r="G84">
+        <v>62</v>
+      </c>
+      <c r="J84">
+        <v>1.02557E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>28</v>
+      </c>
+      <c r="B85">
+        <v>8.6344619999999997E-2</v>
+      </c>
+      <c r="D85">
+        <v>7.0669990000000002E-2</v>
+      </c>
+      <c r="G85">
+        <v>33</v>
+      </c>
+      <c r="J85">
+        <v>2.27973E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86">
+        <v>3.24436E-3</v>
+      </c>
+      <c r="J86">
+        <v>1.3443500000000001E-2</v>
+      </c>
+      <c r="K86">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>29</v>
+      </c>
+      <c r="B87">
+        <v>1.561766E-2</v>
+      </c>
+      <c r="D87">
+        <v>1.337354E-2</v>
+      </c>
+      <c r="E87">
+        <v>7.21</v>
+      </c>
+      <c r="J87">
+        <v>4.3497399999999999E-2</v>
+      </c>
+      <c r="K87">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>30</v>
+      </c>
+      <c r="B88">
+        <v>8.386101E-2</v>
+      </c>
+      <c r="D88">
+        <v>0.10148158</v>
+      </c>
+      <c r="E88">
+        <v>17.36</v>
+      </c>
+      <c r="F88">
+        <v>66</v>
+      </c>
+      <c r="G88">
+        <v>209</v>
+      </c>
+      <c r="J88">
+        <v>6.9922999999999999E-2</v>
+      </c>
+      <c r="K88">
+        <v>143.69999999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89">
+        <v>2.3941100000000001E-3</v>
+      </c>
+      <c r="D89">
+        <v>4.7200699999999998E-3</v>
+      </c>
+      <c r="H89">
+        <v>7.2</v>
+      </c>
+      <c r="I89">
+        <v>2</v>
+      </c>
+      <c r="J89">
+        <v>3.3560000000000003E-4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>125</v>
+      </c>
+      <c r="B90">
+        <v>2.5954900000000002E-3</v>
+      </c>
+      <c r="C90">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="I90">
+        <v>2.6</v>
+      </c>
+      <c r="J90">
+        <v>1.552E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>31</v>
+      </c>
+      <c r="B91">
+        <v>3.9648269999999999E-2</v>
+      </c>
+      <c r="C91">
+        <v>0.22570000000000001</v>
+      </c>
+      <c r="D91">
+        <v>2.4911500000000001E-3</v>
+      </c>
+      <c r="G91">
+        <v>21</v>
+      </c>
+      <c r="H91">
+        <v>2.34</v>
+      </c>
+      <c r="J91">
+        <v>1.0234699999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4228,7 +5617,7 @@
         <v>62</v>
       </c>
       <c r="C65">
-        <f t="shared" ref="C65:C96" si="2">B65/$E$1</f>
+        <f t="shared" ref="C65:C79" si="2">B65/$E$1</f>
         <v>1.3872418499541316E-3</v>
       </c>
     </row>
@@ -4410,7 +5799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -4493,7 +5882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
@@ -5080,7 +6469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -5147,11 +6536,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>

</xml_diff>